<commit_message>
Minor change to protocol definition
</commit_message>
<xml_diff>
--- a/serial_protocols_definition.xlsx
+++ b/serial_protocols_definition.xlsx
@@ -231,16 +231,16 @@
     <t>Same technique if ESC character is also accidentally present in data, it must be escaped as well</t>
   </si>
   <si>
-    <t>return variable value</t>
-  </si>
-  <si>
     <t>write to variable</t>
   </si>
   <si>
-    <t>get  variable table</t>
-  </si>
-  <si>
-    <t>SLAVE SIDE</t>
+    <t>get/return variable value</t>
+  </si>
+  <si>
+    <t>get/return  variable table</t>
+  </si>
+  <si>
+    <t>MASTER/SLAVE</t>
   </si>
 </sst>
 </file>
@@ -548,6 +548,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -560,8 +563,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -597,25 +615,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -953,10 +953,10 @@
       <c r="C11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="E11" s="31"/>
       <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1184,10 +1184,10 @@
       <c r="B24" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="C24" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="31"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="16"/>
       <c r="F24" s="24" t="s">
         <v>60</v>
@@ -1203,14 +1203,14 @@
       </c>
       <c r="J24" s="17"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="33" t="s">
+      <c r="L24" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
@@ -1244,10 +1244,10 @@
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="22"/>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="32"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="16"/>
@@ -1263,8 +1263,8 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="22"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="16"/>
@@ -1282,22 +1282,22 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="30"/>
       <c r="F30" s="24" t="s">
         <v>60</v>
       </c>
@@ -1312,38 +1312,38 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1364,12 +1364,13 @@
   <dimension ref="B7:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1398,10 +1399,10 @@
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
       <c r="R8" s="15"/>
       <c r="S8" s="17"/>
     </row>
@@ -1415,15 +1416,15 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="50" t="s">
+      <c r="F9" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="44" t="s">
+      <c r="G9" s="36"/>
+      <c r="H9" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
@@ -1458,14 +1459,14 @@
       <c r="B11" s="7"/>
       <c r="C11" s="20"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
@@ -1479,10 +1480,10 @@
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="48"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1492,32 +1493,32 @@
       <c r="I14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="47" t="s">
+      <c r="J14" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="47"/>
+      <c r="K14" s="51"/>
       <c r="L14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N14" s="36" t="s">
+      <c r="N14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="38" t="s">
+      <c r="O14" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="40"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="46"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="46"/>
+      <c r="D15" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="39"/>
       <c r="F15" s="6" t="s">
         <v>24</v>
       </c>
@@ -1527,28 +1528,28 @@
       <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="45" t="s">
+      <c r="J15" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="45"/>
+      <c r="K15" s="38"/>
       <c r="L15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="N15" s="37"/>
-      <c r="O15" s="41" t="s">
+      <c r="N15" s="43"/>
+      <c r="O15" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="43"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="49"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="46"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="39"/>
       <c r="F16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1558,21 +1559,21 @@
       <c r="I16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="45" t="s">
+      <c r="J16" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="45"/>
+      <c r="K16" s="38"/>
       <c r="L16" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="46" t="s">
+      <c r="C17" s="34"/>
+      <c r="D17" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="46"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1582,10 +1583,10 @@
       <c r="I17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="45" t="s">
+      <c r="J17" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="45"/>
+      <c r="K17" s="38"/>
       <c r="L17" s="5" t="s">
         <v>56</v>
       </c>
@@ -1597,10 +1598,10 @@
       <c r="I18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="45" t="s">
+      <c r="J18" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="45"/>
+      <c r="K18" s="38"/>
       <c r="L18" s="5" t="s">
         <v>54</v>
       </c>
@@ -1612,10 +1613,10 @@
       <c r="I19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="45" t="s">
+      <c r="J19" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="45"/>
+      <c r="K19" s="38"/>
       <c r="L19" s="5" t="s">
         <v>55</v>
       </c>
@@ -1627,10 +1628,10 @@
       <c r="I20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="45" t="s">
+      <c r="J20" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="45"/>
+      <c r="K20" s="38"/>
       <c r="L20" s="5" t="s">
         <v>56</v>
       </c>
@@ -1642,10 +1643,10 @@
       <c r="I21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="45" t="s">
+      <c r="J21" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="45"/>
+      <c r="K21" s="38"/>
       <c r="L21" s="5" t="s">
         <v>54</v>
       </c>
@@ -1657,10 +1658,10 @@
       <c r="I22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="34" t="s">
+      <c r="J22" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="K22" s="35"/>
+      <c r="K22" s="41"/>
       <c r="L22" s="5" t="s">
         <v>57</v>
       </c>
@@ -1671,6 +1672,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="F9:G9"/>
@@ -1683,17 +1691,10 @@
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
     <mergeCell ref="N14:N15"/>
     <mergeCell ref="O14:R14"/>
     <mergeCell ref="O15:R15"/>
     <mergeCell ref="H9:J9"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J14:K14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Future improvements on logger protocol
</commit_message>
<xml_diff>
--- a/serial_protocols_definition.xlsx
+++ b/serial_protocols_definition.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
   <si>
     <t>command</t>
   </si>
@@ -262,13 +262,64 @@
   </si>
   <si>
     <t>37B</t>
+  </si>
+  <si>
+    <t>get command tells the MCU to return variable at specified delay</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>MCU stops sending var</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>50 ms</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>100 ms</t>
+  </si>
+  <si>
+    <t>10 ms</t>
+  </si>
+  <si>
+    <t>0xX0</t>
+  </si>
+  <si>
+    <t>0x30</t>
+  </si>
+  <si>
+    <t>0x40</t>
+  </si>
+  <si>
+    <t>500 ms</t>
+  </si>
+  <si>
+    <t>250 ms</t>
+  </si>
+  <si>
+    <t>0x50</t>
+  </si>
+  <si>
+    <t>0x60</t>
+  </si>
+  <si>
+    <t>NO DONE YET</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,8 +335,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +380,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -516,10 +579,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -591,71 +655,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1400,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1436,10 +1505,10 @@
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+      <c r="P8" s="35"/>
+      <c r="Q8" s="35"/>
       <c r="R8" s="15"/>
       <c r="S8" s="17"/>
     </row>
@@ -1453,15 +1522,15 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="51"/>
-      <c r="H9" s="46" t="s">
+      <c r="G9" s="36"/>
+      <c r="H9" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
@@ -1517,10 +1586,10 @@
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
-      <c r="D14" s="52" t="s">
+      <c r="D14" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="52"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1530,34 +1599,34 @@
       <c r="I14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="42" t="s">
+      <c r="J14" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="42"/>
+      <c r="K14" s="50"/>
       <c r="L14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="54" t="s">
+      <c r="N14" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="39" t="s">
+      <c r="O14" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="40"/>
-      <c r="Q14" s="40"/>
-      <c r="R14" s="41"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="49"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="49" t="s">
+      <c r="C15" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="53" t="s">
+      <c r="D15" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="53"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="6" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1565,28 +1634,28 @@
       <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="35" t="s">
+      <c r="J15" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="35"/>
+      <c r="K15" s="42"/>
       <c r="L15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="55"/>
-      <c r="O15" s="43" t="s">
+      <c r="N15" s="45"/>
+      <c r="O15" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="P15" s="44"/>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="45"/>
+      <c r="P15" s="52"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="53"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="53" t="s">
+      <c r="C16" s="40"/>
+      <c r="D16" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="53"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1596,21 +1665,21 @@
       <c r="I16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="35" t="s">
+      <c r="J16" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="35"/>
+      <c r="K16" s="42"/>
       <c r="L16" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="53" t="s">
+      <c r="C17" s="40"/>
+      <c r="D17" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="53"/>
+      <c r="E17" s="43"/>
       <c r="F17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1620,10 +1689,10 @@
       <c r="I17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="35" t="s">
+      <c r="J17" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="35"/>
+      <c r="K17" s="42"/>
       <c r="L17" s="5" t="s">
         <v>55</v>
       </c>
@@ -1635,10 +1704,10 @@
       <c r="I18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="35" t="s">
+      <c r="J18" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="35"/>
+      <c r="K18" s="42"/>
       <c r="L18" s="5" t="s">
         <v>53</v>
       </c>
@@ -1650,64 +1719,135 @@
       <c r="I19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="35" t="s">
+      <c r="J19" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="35"/>
+      <c r="K19" s="42"/>
       <c r="L19" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D20" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="57"/>
       <c r="H20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="35" t="s">
+      <c r="J20" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="35"/>
+      <c r="K20" s="42"/>
       <c r="L20" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D21" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>80</v>
+      </c>
       <c r="H21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="35"/>
+      <c r="K21" s="42"/>
       <c r="L21" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C22" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" t="s">
+        <v>82</v>
+      </c>
       <c r="H22" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="36" t="s">
+      <c r="J22" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="K22" s="37"/>
+      <c r="K22" s="55"/>
       <c r="L22" s="5" t="s">
         <v>78</v>
       </c>
     </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C23" s="56"/>
+      <c r="D23" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C24" s="56"/>
+      <c r="D24" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C25" s="56"/>
+      <c r="D25" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D26" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D27" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="57" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="I28" s="48" t="s">
+      <c r="D28" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="I28" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="J28" s="48"/>
+      <c r="J28" s="39"/>
       <c r="K28" s="29" t="s">
         <v>2</v>
       </c>
@@ -1736,19 +1876,19 @@
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
       <c r="K29" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L29" s="47" t="s">
+      <c r="L29" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="M29" s="47"/>
-      <c r="N29" s="47" t="s">
+      <c r="M29" s="38"/>
+      <c r="N29" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O29" s="47"/>
+      <c r="O29" s="38"/>
       <c r="P29" s="29" t="s">
         <v>74</v>
       </c>
@@ -1760,42 +1900,46 @@
       </c>
     </row>
     <row r="31" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="38" t="s">
+      <c r="K31" s="46" t="s">
         <v>70</v>
       </c>
-      <c r="L31" s="38"/>
+      <c r="L31" s="46"/>
       <c r="N31" s="19"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K32" s="38"/>
-      <c r="L32" s="38"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="46"/>
       <c r="N32" s="19"/>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
       <c r="N33" s="19"/>
     </row>
     <row r="34" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K34" s="38"/>
-      <c r="L34" s="38"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
     </row>
     <row r="35" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K35" s="38"/>
-      <c r="L35" s="38"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
     </row>
     <row r="36" spans="11:14" x14ac:dyDescent="0.25">
       <c r="L36" s="19"/>
       <c r="M36" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="H9:J9"/>
+  <mergeCells count="28">
+    <mergeCell ref="K31:L35"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="I28:J29"/>
@@ -1807,16 +1951,13 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="N14:N15"/>
-    <mergeCell ref="K31:L35"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="H9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SOF char is now different from EOF
Solved #6
</commit_message>
<xml_diff>
--- a/serial_protocols_definition.xlsx
+++ b/serial_protocols_definition.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="serial protocol" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>command</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>NO DONE YET</t>
+  </si>
+  <si>
+    <t>0xF7</t>
   </si>
 </sst>
 </file>
@@ -640,6 +643,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -655,6 +659,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -664,64 +725,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
@@ -1011,8 +1014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:R38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,10 +1062,10 @@
       <c r="C11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="32"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1168,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>11</v>
@@ -1290,10 +1293,10 @@
       <c r="B24" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="33"/>
+      <c r="D24" s="34"/>
       <c r="E24" s="16"/>
       <c r="F24" s="24" t="s">
         <v>58</v>
@@ -1309,14 +1312,14 @@
       </c>
       <c r="J24" s="17"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="30" t="s">
+      <c r="L24" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="16"/>
@@ -1350,10 +1353,10 @@
     <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="22"/>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="34"/>
+      <c r="D26" s="35"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="16"/>
@@ -1369,8 +1372,8 @@
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="22"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="16"/>
@@ -1388,22 +1391,22 @@
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="31"/>
+      <c r="D30" s="32"/>
       <c r="F30" s="24" t="s">
         <v>58</v>
       </c>
@@ -1418,38 +1421,38 @@
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
     </row>
     <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="31"/>
+      <c r="D34" s="32"/>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1469,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -1505,10 +1508,10 @@
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
+      <c r="N8" s="55"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="55"/>
       <c r="R8" s="15"/>
       <c r="S8" s="17"/>
     </row>
@@ -1522,15 +1525,15 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37" t="s">
+      <c r="G9" s="56"/>
+      <c r="H9" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
@@ -1565,14 +1568,14 @@
       <c r="B11" s="7"/>
       <c r="C11" s="20"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
       <c r="M11" s="19"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
@@ -1586,10 +1589,10 @@
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="15"/>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="41"/>
+      <c r="E14" s="50"/>
       <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1599,32 +1602,32 @@
       <c r="I14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="50" t="s">
+      <c r="J14" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="50"/>
+      <c r="K14" s="41"/>
       <c r="L14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="44" t="s">
+      <c r="N14" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="47" t="s">
+      <c r="O14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="49"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="39"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="6" t="s">
         <v>88</v>
       </c>
@@ -1634,28 +1637,28 @@
       <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="42"/>
+      <c r="K15" s="40"/>
       <c r="L15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N15" s="45"/>
-      <c r="O15" s="51" t="s">
+      <c r="N15" s="53"/>
+      <c r="O15" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="52"/>
-      <c r="R15" s="53"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="44"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="49"/>
+      <c r="D16" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1665,21 +1668,21 @@
       <c r="I16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="42" t="s">
+      <c r="J16" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="42"/>
+      <c r="K16" s="40"/>
       <c r="L16" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="43" t="s">
+      <c r="C17" s="49"/>
+      <c r="D17" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1689,10 +1692,10 @@
       <c r="I17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="42"/>
+      <c r="K17" s="40"/>
       <c r="L17" s="5" t="s">
         <v>55</v>
       </c>
@@ -1704,10 +1707,10 @@
       <c r="I18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="42" t="s">
+      <c r="J18" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="42"/>
+      <c r="K18" s="40"/>
       <c r="L18" s="5" t="s">
         <v>53</v>
       </c>
@@ -1719,38 +1722,38 @@
       <c r="I19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="42" t="s">
+      <c r="J19" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="42"/>
+      <c r="K19" s="40"/>
       <c r="L19" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="E20" s="57"/>
+      <c r="E20" s="30"/>
       <c r="H20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="42" t="s">
+      <c r="J20" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="42"/>
+      <c r="K20" s="40"/>
       <c r="L20" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D21" s="57" t="s">
+      <c r="D21" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="30" t="s">
         <v>80</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -1759,22 +1762,22 @@
       <c r="I21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="42" t="s">
+      <c r="J21" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="42"/>
+      <c r="K21" s="40"/>
       <c r="L21" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C22" s="56" t="s">
+      <c r="C22" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="D22" s="57" t="s">
+      <c r="D22" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="30" t="s">
         <v>81</v>
       </c>
       <c r="F22" t="s">
@@ -1786,68 +1789,68 @@
       <c r="I22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="54" t="s">
+      <c r="J22" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="K22" s="55"/>
+      <c r="K22" s="46"/>
       <c r="L22" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C23" s="56"/>
-      <c r="D23" s="57" t="s">
+      <c r="C23" s="54"/>
+      <c r="D23" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="30" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="56"/>
-      <c r="D24" s="57" t="s">
+      <c r="C24" s="54"/>
+      <c r="D24" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="57" t="s">
+      <c r="E24" s="30" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C25" s="56"/>
-      <c r="D25" s="57" t="s">
+      <c r="C25" s="54"/>
+      <c r="D25" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="57" t="s">
+      <c r="E25" s="30" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D26" s="57" t="s">
+      <c r="D26" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="57" t="s">
+      <c r="E26" s="30" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D27" s="57" t="s">
+      <c r="D27" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="30" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D28" s="57" t="s">
+      <c r="D28" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="39" t="s">
+      <c r="I28" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="J28" s="39"/>
+      <c r="J28" s="48"/>
       <c r="K28" s="29" t="s">
         <v>2</v>
       </c>
@@ -1876,19 +1879,19 @@
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
       <c r="K29" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L29" s="38" t="s">
+      <c r="L29" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="M29" s="38"/>
-      <c r="N29" s="38" t="s">
+      <c r="M29" s="47"/>
+      <c r="N29" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="O29" s="38"/>
+      <c r="O29" s="47"/>
       <c r="P29" s="29" t="s">
         <v>74</v>
       </c>
@@ -1900,29 +1903,29 @@
       </c>
     </row>
     <row r="31" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="46" t="s">
+      <c r="K31" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="L31" s="46"/>
+      <c r="L31" s="36"/>
       <c r="N31" s="19"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K32" s="46"/>
-      <c r="L32" s="46"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
       <c r="N32" s="19"/>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
       <c r="N33" s="19"/>
     </row>
     <row r="34" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K34" s="46"/>
-      <c r="L34" s="46"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
     </row>
     <row r="35" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K35" s="46"/>
-      <c r="L35" s="46"/>
+      <c r="K35" s="36"/>
+      <c r="L35" s="36"/>
     </row>
     <row r="36" spans="11:14" x14ac:dyDescent="0.25">
       <c r="L36" s="19"/>
@@ -1930,6 +1933,20 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="K31:L35"/>
     <mergeCell ref="O14:R14"/>
     <mergeCell ref="J17:K17"/>
@@ -1943,21 +1960,7 @@
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="I28:J29"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
     <mergeCell ref="N14:N15"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="H9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed array_size in octets for table entry
Program does not changes
</commit_message>
<xml_diff>
--- a/serial_protocols_definition.xlsx
+++ b/serial_protocols_definition.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B48923\Documents\GitHub\Freescale_Cup\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10440" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="serial protocol" sheetId="2" r:id="rId1"/>
     <sheet name="logger protocol" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -243,9 +238,6 @@
     <t>TABLE ENTRY STRUCTURE</t>
   </si>
   <si>
-    <t>array_size</t>
-  </si>
-  <si>
     <t>byte 5</t>
   </si>
   <si>
@@ -319,13 +311,16 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>size_octets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,6 +657,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -680,57 +720,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Insatisfaisant" xfId="1" builtinId="27"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -795,7 +790,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -830,7 +825,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1007,21 +1002,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A8:R38"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
@@ -1031,8 +1026,8 @@
     <col min="12" max="12" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" ht="15.75" thickBot="1"/>
+    <row r="9" spans="2:18" ht="15.75" thickBot="1">
       <c r="C9" s="11" t="s">
         <v>2</v>
       </c>
@@ -1058,7 +1053,7 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18">
       <c r="B11" s="7" t="s">
         <v>42</v>
       </c>
@@ -1084,7 +1079,7 @@
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="14"/>
@@ -1102,7 +1097,7 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18">
       <c r="B13" s="7"/>
       <c r="C13" s="20"/>
       <c r="D13" s="14"/>
@@ -1121,7 +1116,7 @@
       <c r="Q13" s="15"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18">
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="G14" s="16"/>
@@ -1136,7 +1131,7 @@
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18">
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
@@ -1149,7 +1144,7 @@
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -1169,12 +1164,12 @@
       <c r="P16" s="15"/>
       <c r="Q16" s="16"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="B17" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>11</v>
@@ -1191,7 +1186,7 @@
       <c r="P17" s="15"/>
       <c r="Q17" s="16"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1208,7 @@
       <c r="P18" s="15"/>
       <c r="Q18" s="16"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
@@ -1235,7 +1230,7 @@
       <c r="P19" s="15"/>
       <c r="Q19" s="16"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="17"/>
@@ -1248,7 +1243,7 @@
       <c r="P20" s="15"/>
       <c r="Q20" s="16"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="I21" s="17"/>
@@ -1261,7 +1256,7 @@
       <c r="P21" s="16"/>
       <c r="Q21" s="16"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="B22" s="2" t="s">
         <v>41</v>
       </c>
@@ -1281,7 +1276,7 @@
       <c r="P22" s="16"/>
       <c r="Q22" s="16"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="J23" s="17"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16"/>
@@ -1291,7 +1286,7 @@
       <c r="P23" s="16"/>
       <c r="Q23" s="16"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" s="16"/>
       <c r="B24" s="16" t="s">
         <v>56</v>
@@ -1324,7 +1319,7 @@
       <c r="P24" s="31"/>
       <c r="Q24" s="31"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" s="16"/>
       <c r="C25" s="1" t="s">
         <v>61</v>
@@ -1353,7 +1348,7 @@
       <c r="P25" s="16"/>
       <c r="Q25" s="16"/>
     </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="15" customHeight="1">
       <c r="A26" s="16"/>
       <c r="B26" s="22"/>
       <c r="C26" s="35" t="s">
@@ -1372,7 +1367,7 @@
       <c r="P26" s="16"/>
       <c r="Q26" s="16"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" s="16"/>
       <c r="B27" s="22"/>
       <c r="C27" s="35"/>
@@ -1391,7 +1386,7 @@
       <c r="P27" s="16"/>
       <c r="Q27" s="16"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="35"/>
@@ -1401,11 +1396,11 @@
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="C30" s="32" t="s">
         <v>64</v>
       </c>
@@ -1423,37 +1418,37 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4">
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
     </row>
-    <row r="34" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" ht="15" customHeight="1">
       <c r="C34" s="32" t="s">
         <v>65</v>
       </c>
       <c r="D34" s="32"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4">
       <c r="C35" s="32"/>
       <c r="D35" s="32"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4">
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4">
       <c r="C37" s="32"/>
       <c r="D37" s="32"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4">
       <c r="C38" s="32"/>
       <c r="D38" s="32"/>
     </row>
@@ -1472,22 +1467,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B7:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:19" ht="15.75" thickBot="1"/>
+    <row r="8" spans="2:19" ht="15.75" thickBot="1">
       <c r="D8" s="11" t="s">
         <v>2</v>
       </c>
@@ -1511,14 +1506,14 @@
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="37"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
       <c r="R8" s="15"/>
       <c r="S8" s="17"/>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19">
       <c r="C9" s="7" t="s">
         <v>44</v>
       </c>
@@ -1528,15 +1523,15 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="39" t="s">
+      <c r="G9" s="53"/>
+      <c r="H9" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="25"/>
       <c r="L9" s="26"/>
       <c r="M9" s="26"/>
@@ -1547,7 +1542,7 @@
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -1567,7 +1562,7 @@
       <c r="R10" s="15"/>
       <c r="S10" s="15"/>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19">
       <c r="B11" s="7"/>
       <c r="C11" s="20"/>
       <c r="D11" s="14"/>
@@ -1586,16 +1581,16 @@
       <c r="Q11" s="15"/>
       <c r="R11" s="15"/>
     </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19">
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:19">
       <c r="B14" s="15"/>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="41"/>
+      <c r="E14" s="56"/>
       <c r="F14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1605,34 +1600,34 @@
       <c r="I14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="48" t="s">
+      <c r="J14" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="48"/>
+      <c r="K14" s="41"/>
       <c r="L14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="56" t="s">
+      <c r="N14" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="45" t="s">
+      <c r="O14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="46"/>
-      <c r="R14" s="47"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="39"/>
+    </row>
+    <row r="15" spans="2:19">
       <c r="B15" s="15"/>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="43"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1640,31 +1635,31 @@
       <c r="I15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="K15" s="42"/>
+      <c r="K15" s="40"/>
       <c r="L15" s="5" t="s">
         <v>53</v>
       </c>
       <c r="M15" t="s">
-        <v>97</v>
-      </c>
-      <c r="N15" s="57"/>
-      <c r="O15" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="N15" s="50"/>
+      <c r="O15" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="51"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="44"/>
+    </row>
+    <row r="16" spans="2:19">
       <c r="B16" s="15"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="55"/>
+      <c r="D16" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="43"/>
+      <c r="E16" s="57"/>
       <c r="F16" s="6" t="s">
         <v>26</v>
       </c>
@@ -1674,21 +1669,21 @@
       <c r="I16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J16" s="42" t="s">
+      <c r="J16" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="42"/>
+      <c r="K16" s="40"/>
       <c r="L16" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18">
       <c r="B17" s="15"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="43" t="s">
+      <c r="C17" s="55"/>
+      <c r="D17" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="43"/>
+      <c r="E17" s="57"/>
       <c r="F17" s="6" t="s">
         <v>27</v>
       </c>
@@ -1698,53 +1693,53 @@
       <c r="I17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="42"/>
+      <c r="K17" s="40"/>
       <c r="L17" s="5" t="s">
         <v>55</v>
       </c>
       <c r="M17" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18">
       <c r="H18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="42" t="s">
+      <c r="J18" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="K18" s="42"/>
+      <c r="K18" s="40"/>
       <c r="L18" s="5" t="s">
         <v>53</v>
       </c>
       <c r="M18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18">
       <c r="H19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="42" t="s">
+      <c r="J19" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="42"/>
+      <c r="K19" s="40"/>
       <c r="L19" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18">
       <c r="D20" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E20" s="30"/>
       <c r="H20" s="3" t="s">
@@ -1753,20 +1748,20 @@
       <c r="I20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J20" s="42" t="s">
+      <c r="J20" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="K20" s="42"/>
+      <c r="K20" s="40"/>
       <c r="L20" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18">
       <c r="D21" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>23</v>
@@ -1774,29 +1769,29 @@
       <c r="I21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="42" t="s">
+      <c r="J21" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="42"/>
+      <c r="K21" s="40"/>
       <c r="L21" s="5" t="s">
         <v>53</v>
       </c>
       <c r="M21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C22" s="36" t="s">
-        <v>79</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18">
+      <c r="C22" s="51" t="s">
+        <v>78</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>24</v>
       </c>
       <c r="E22" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" t="s">
         <v>81</v>
-      </c>
-      <c r="F22" t="s">
-        <v>82</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>36</v>
@@ -1804,68 +1799,68 @@
       <c r="I22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J22" s="52" t="s">
+      <c r="J22" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="K22" s="46"/>
+      <c r="L22" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="K22" s="53"/>
-      <c r="L22" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C23" s="36"/>
+    </row>
+    <row r="23" spans="2:18">
+      <c r="C23" s="51"/>
       <c r="D23" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18">
+      <c r="C24" s="51"/>
+      <c r="D24" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="E23" s="30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C24" s="36"/>
-      <c r="D24" s="30" t="s">
+    </row>
+    <row r="25" spans="2:18">
+      <c r="C25" s="51"/>
+      <c r="D25" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C25" s="36"/>
-      <c r="D25" s="30" t="s">
+    </row>
+    <row r="26" spans="2:18">
+      <c r="D26" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="30" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D26" s="30" t="s">
+      <c r="E26" s="30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18">
+      <c r="D27" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="E26" s="30" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D27" s="30" t="s">
+    </row>
+    <row r="28" spans="2:18">
+      <c r="D28" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D28" s="30" t="s">
-        <v>94</v>
-      </c>
       <c r="E28" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="I28" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="I28" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="J28" s="55"/>
+      <c r="J28" s="48"/>
       <c r="K28" s="29" t="s">
         <v>2</v>
       </c>
@@ -1882,72 +1877,86 @@
         <v>35</v>
       </c>
       <c r="P28" s="29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q28" s="29" t="s">
         <v>38</v>
       </c>
       <c r="R28" s="29" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
       <c r="K29" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="L29" s="54" t="s">
+      <c r="L29" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="O29" s="54"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="O29" s="47"/>
       <c r="P29" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q29" s="29" t="s">
         <v>38</v>
       </c>
       <c r="R29" s="29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K31" s="44" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" ht="15" customHeight="1">
+      <c r="K31" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="L31" s="44"/>
+      <c r="L31" s="36"/>
       <c r="N31" s="19"/>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
+    <row r="32" spans="2:18">
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
       <c r="N32" s="19"/>
     </row>
-    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K33" s="44"/>
-      <c r="L33" s="44"/>
+    <row r="33" spans="11:14">
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
       <c r="N33" s="19"/>
     </row>
-    <row r="34" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K34" s="44"/>
-      <c r="L34" s="44"/>
-    </row>
-    <row r="35" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-    </row>
-    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:14">
+      <c r="K34" s="36"/>
+      <c r="L34" s="36"/>
+    </row>
+    <row r="35" spans="11:14">
+      <c r="K35" s="36"/>
+      <c r="L35" s="36"/>
+    </row>
+    <row r="36" spans="11:14">
       <c r="L36" s="19"/>
       <c r="M36" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
     <mergeCell ref="K31:L35"/>
     <mergeCell ref="O14:R14"/>
     <mergeCell ref="J17:K17"/>
@@ -1962,20 +1971,6 @@
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="I28:J29"/>
     <mergeCell ref="N14:N15"/>
-    <mergeCell ref="C22:C25"/>
-    <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>